<commit_message>
Update system inputs from Excel
</commit_message>
<xml_diff>
--- a/inputData/eco_system_inputs_FG_example.xlsx
+++ b/inputData/eco_system_inputs_FG_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10791792_polimi_it/Documents/2024-04 Economic model/EcoModel/inputData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-Eco\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="11_F25DC773A252ABDACC1048D3711B4E545ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0242D2BD-84E2-4BA8-95E5-4C2C0B00E366}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50204952-7B6D-48A6-AD04-94375ADF5722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atm" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>structure.m</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>R0</t>
+  </si>
+  <si>
+    <t>batt.E_rated</t>
+  </si>
+  <si>
+    <t>batt.f_repl</t>
   </si>
 </sst>
 </file>
@@ -421,12 +427,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -443,16 +449,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B3DA40-233C-46C9-8316-C78F88E0B4B1}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +466,7 @@
         <v>122.5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -468,7 +474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -476,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -484,19 +490,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
   </sheetData>
@@ -512,13 +518,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -526,7 +532,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -534,7 +540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -542,7 +548,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -550,16 +556,16 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
   </sheetData>
@@ -572,16 +578,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -589,7 +595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -597,7 +603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -605,7 +611,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -613,7 +619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -628,19 +634,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B061E06-0D80-41AB-A869-146906050ACA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -648,11 +654,27 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
         <v>-1</v>
       </c>
     </row>

</xml_diff>